<commit_message>
Fixed some bugs in assessment page
</commit_message>
<xml_diff>
--- a/SGP_Mitra-main/app/data/Clinical_Data/Final_DS_2.xlsx
+++ b/SGP_Mitra-main/app/data/Clinical_Data/Final_DS_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smit\Desktop\DESKTOP\6th sem\New SGP\Mitra_Dhruvil_Branch\SGP_Mitra\SGP_Mitra-main\app\data\Clinical_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smit\Desktop\DESKTOP\Github Repos\SGP_Mitra\SGP_Mitra-main\app\data\Clinical_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFA45B3-36AC-4955-B203-40466AC2B45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6879535C-655E-4486-BA3C-9FFA4FE284F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1488,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1665,7 +1665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>

</xml_diff>